<commit_message>
Add 2 xls files for some calculations, fix Vector::getDotProduct() API doc.
</commit_message>
<xml_diff>
--- a/PGE/PRRE/docpages/internal/PR00FPSvsPRRE-Transformations.xlsx
+++ b/PGE/PRRE/docpages/internal/PR00FPSvsPRRE-Transformations.xlsx
@@ -177,9 +177,6 @@
     <t>v4'''''</t>
   </si>
   <si>
-    <t>Input values above ... Do NOT modify anything below!</t>
-  </si>
-  <si>
     <t>Tr done with negated x,y cam pos!</t>
   </si>
   <si>
@@ -259,6 +256,9 @@
   </si>
   <si>
     <t xml:space="preserve">temp </t>
+  </si>
+  <si>
+    <t>Input values above ... Do NOT modify anything below!             --- Sheet made by PRooF88 ---</t>
   </si>
 </sst>
 </file>
@@ -842,7 +842,67 @@
     <xf numFmtId="165" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="6" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -853,18 +913,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -880,54 +928,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1082,11 +1082,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="91583232"/>
-        <c:axId val="91584768"/>
+        <c:axId val="97010432"/>
+        <c:axId val="97011968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91583232"/>
+        <c:axId val="97010432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="800"/>
@@ -1095,12 +1095,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91584768"/>
+        <c:crossAx val="97011968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="91584768"/>
+        <c:axId val="97011968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="600"/>
@@ -1110,7 +1110,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91583232"/>
+        <c:crossAx val="97010432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1119,7 +1119,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1184,11 +1184,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="91608192"/>
-        <c:axId val="91609728"/>
+        <c:axId val="62280832"/>
+        <c:axId val="62282368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91608192"/>
+        <c:axId val="62280832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="800"/>
@@ -1197,12 +1197,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91609728"/>
+        <c:crossAx val="62282368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="91609728"/>
+        <c:axId val="62282368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="600"/>
@@ -1212,7 +1212,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91608192"/>
+        <c:crossAx val="62280832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1221,7 +1221,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000178" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000178" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1286,11 +1286,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="95696384"/>
-        <c:axId val="95697920"/>
+        <c:axId val="62305792"/>
+        <c:axId val="62307328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="95696384"/>
+        <c:axId val="62305792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="800"/>
@@ -1299,12 +1299,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95697920"/>
+        <c:crossAx val="62307328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="95697920"/>
+        <c:axId val="62307328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="600"/>
@@ -1314,7 +1314,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95696384"/>
+        <c:crossAx val="62305792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1323,7 +1323,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1712,8 +1712,8 @@
   <dimension ref="A1:AH125"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1755,22 +1755,22 @@
       </c>
       <c r="E1" s="62"/>
       <c r="F1" s="62"/>
-      <c r="G1" s="109" t="s">
-        <v>72</v>
-      </c>
-      <c r="H1" s="109"/>
-      <c r="I1" s="109"/>
-      <c r="J1" s="109"/>
-      <c r="K1" s="109"/>
-      <c r="L1" s="109"/>
-      <c r="M1" s="109"/>
-      <c r="N1" s="109"/>
-      <c r="O1" s="109"/>
-      <c r="P1" s="109"/>
-      <c r="Q1" s="109"/>
-      <c r="R1" s="109"/>
-      <c r="S1" s="109"/>
-      <c r="T1" s="109"/>
+      <c r="G1" s="122" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" s="122"/>
+      <c r="I1" s="122"/>
+      <c r="J1" s="122"/>
+      <c r="K1" s="122"/>
+      <c r="L1" s="122"/>
+      <c r="M1" s="122"/>
+      <c r="N1" s="122"/>
+      <c r="O1" s="122"/>
+      <c r="P1" s="122"/>
+      <c r="Q1" s="122"/>
+      <c r="R1" s="122"/>
+      <c r="S1" s="122"/>
+      <c r="T1" s="122"/>
       <c r="U1" s="62"/>
       <c r="V1" s="62"/>
       <c r="W1" s="62"/>
@@ -1809,21 +1809,21 @@
       <c r="M2" s="30"/>
       <c r="N2" s="30"/>
       <c r="O2" s="30"/>
-      <c r="P2" s="131" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q2" s="131"/>
+      <c r="P2" s="107" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q2" s="107"/>
       <c r="R2" s="30"/>
-      <c r="S2" s="131" t="s">
-        <v>66</v>
-      </c>
-      <c r="T2" s="131"/>
+      <c r="S2" s="107" t="s">
+        <v>65</v>
+      </c>
+      <c r="T2" s="107"/>
       <c r="U2" s="30"/>
       <c r="V2" s="30"/>
-      <c r="W2" s="102" t="s">
-        <v>75</v>
-      </c>
-      <c r="X2" s="102"/>
+      <c r="W2" s="105" t="s">
+        <v>74</v>
+      </c>
+      <c r="X2" s="105"/>
       <c r="Y2" s="30"/>
       <c r="Z2" s="30"/>
       <c r="AA2" s="30"/>
@@ -1849,25 +1849,25 @@
       </c>
       <c r="E3" s="30"/>
       <c r="F3" s="30"/>
-      <c r="G3" s="104" t="s">
+      <c r="G3" s="124" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="105"/>
-      <c r="I3" s="105"/>
+      <c r="H3" s="125"/>
+      <c r="I3" s="125"/>
       <c r="J3" s="43">
         <v>80</v>
       </c>
       <c r="K3" s="30"/>
-      <c r="L3" s="104" t="s">
+      <c r="L3" s="124" t="s">
         <v>43</v>
       </c>
-      <c r="M3" s="105"/>
+      <c r="M3" s="125"/>
       <c r="N3" s="46">
         <v>0</v>
       </c>
       <c r="O3" s="30"/>
       <c r="P3" s="49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q3" s="16">
         <f>$J$5 * TAN($J$3 * PI() / 360)</f>
@@ -1875,7 +1875,7 @@
       </c>
       <c r="R3" s="30"/>
       <c r="S3" s="47" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="T3" s="21">
         <f>2*$J$5</f>
@@ -1884,7 +1884,7 @@
       <c r="U3" s="30"/>
       <c r="V3" s="30"/>
       <c r="W3" s="72" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="X3" s="38">
         <v>0</v>
@@ -1914,26 +1914,26 @@
       </c>
       <c r="E4" s="30"/>
       <c r="F4" s="30"/>
-      <c r="G4" s="104" t="s">
+      <c r="G4" s="124" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="105"/>
-      <c r="I4" s="105"/>
+      <c r="H4" s="125"/>
+      <c r="I4" s="125"/>
       <c r="J4" s="16">
         <f>$N$5/$N$6</f>
         <v>1.3333333333333333</v>
       </c>
       <c r="K4" s="30"/>
-      <c r="L4" s="104" t="s">
+      <c r="L4" s="124" t="s">
         <v>44</v>
       </c>
-      <c r="M4" s="105"/>
+      <c r="M4" s="125"/>
       <c r="N4" s="46">
         <v>0</v>
       </c>
       <c r="O4" s="30"/>
       <c r="P4" s="48" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q4" s="13">
         <f>$Q$3*$J$4</f>
@@ -1941,7 +1941,7 @@
       </c>
       <c r="R4" s="30"/>
       <c r="S4" s="29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="T4" s="51">
         <f>$Q$4- -$Q$4</f>
@@ -1950,7 +1950,7 @@
       <c r="U4" s="30"/>
       <c r="V4" s="30"/>
       <c r="W4" s="48" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="X4" s="98">
         <v>1</v>
@@ -1980,19 +1980,19 @@
       </c>
       <c r="E5" s="30"/>
       <c r="F5" s="30"/>
-      <c r="G5" s="104" t="s">
+      <c r="G5" s="124" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="105"/>
-      <c r="I5" s="105"/>
+      <c r="H5" s="125"/>
+      <c r="I5" s="125"/>
       <c r="J5" s="44">
         <v>1</v>
       </c>
       <c r="K5" s="30"/>
-      <c r="L5" s="104" t="s">
+      <c r="L5" s="124" t="s">
         <v>45</v>
       </c>
-      <c r="M5" s="105"/>
+      <c r="M5" s="125"/>
       <c r="N5" s="46">
         <v>800</v>
       </c>
@@ -2001,7 +2001,7 @@
       <c r="Q5" s="30"/>
       <c r="R5" s="30"/>
       <c r="S5" s="29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="T5" s="51">
         <f>$Q$3- -$Q$3</f>
@@ -2036,19 +2036,19 @@
       </c>
       <c r="E6" s="30"/>
       <c r="F6" s="30"/>
-      <c r="G6" s="104" t="s">
+      <c r="G6" s="124" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="105"/>
-      <c r="I6" s="105"/>
+      <c r="H6" s="125"/>
+      <c r="I6" s="125"/>
       <c r="J6" s="44">
         <v>10</v>
       </c>
       <c r="K6" s="30"/>
-      <c r="L6" s="110" t="s">
+      <c r="L6" s="126" t="s">
         <v>46</v>
       </c>
-      <c r="M6" s="111"/>
+      <c r="M6" s="127"/>
       <c r="N6" s="46">
         <v>600</v>
       </c>
@@ -2057,7 +2057,7 @@
       <c r="Q6" s="30"/>
       <c r="R6" s="30"/>
       <c r="S6" s="52" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="T6" s="13">
         <f>$J$7</f>
@@ -2092,18 +2092,18 @@
       </c>
       <c r="E7" s="30"/>
       <c r="F7" s="30"/>
-      <c r="G7" s="110" t="s">
+      <c r="G7" s="126" t="s">
         <v>33</v>
       </c>
-      <c r="H7" s="111"/>
-      <c r="I7" s="111"/>
+      <c r="H7" s="127"/>
+      <c r="I7" s="127"/>
       <c r="J7" s="38">
         <f>J6-J5</f>
         <v>9</v>
       </c>
       <c r="K7" s="30"/>
-      <c r="L7" s="112"/>
-      <c r="M7" s="112"/>
+      <c r="L7" s="128"/>
+      <c r="M7" s="128"/>
       <c r="N7" s="30"/>
       <c r="O7" s="30"/>
       <c r="P7" s="30"/>
@@ -2126,41 +2126,41 @@
       <c r="AG7" s="33"/>
     </row>
     <row r="8" spans="1:33" ht="15.75" thickBot="1">
-      <c r="A8" s="113" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="114"/>
-      <c r="C8" s="114"/>
-      <c r="D8" s="114"/>
-      <c r="E8" s="114"/>
-      <c r="F8" s="114"/>
-      <c r="G8" s="114"/>
-      <c r="H8" s="114"/>
-      <c r="I8" s="114"/>
-      <c r="J8" s="114"/>
-      <c r="K8" s="114"/>
-      <c r="L8" s="114"/>
-      <c r="M8" s="114"/>
-      <c r="N8" s="114"/>
-      <c r="O8" s="114"/>
-      <c r="P8" s="114"/>
-      <c r="Q8" s="114"/>
-      <c r="R8" s="114"/>
-      <c r="S8" s="114"/>
-      <c r="T8" s="114"/>
-      <c r="U8" s="114"/>
-      <c r="V8" s="114"/>
-      <c r="W8" s="114"/>
-      <c r="X8" s="114"/>
-      <c r="Y8" s="114"/>
-      <c r="Z8" s="114"/>
-      <c r="AA8" s="114"/>
-      <c r="AB8" s="114"/>
-      <c r="AC8" s="114"/>
-      <c r="AD8" s="114"/>
-      <c r="AE8" s="114"/>
-      <c r="AF8" s="114"/>
-      <c r="AG8" s="115"/>
+      <c r="A8" s="129" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="130"/>
+      <c r="C8" s="130"/>
+      <c r="D8" s="130"/>
+      <c r="E8" s="130"/>
+      <c r="F8" s="130"/>
+      <c r="G8" s="130"/>
+      <c r="H8" s="130"/>
+      <c r="I8" s="130"/>
+      <c r="J8" s="130"/>
+      <c r="K8" s="130"/>
+      <c r="L8" s="130"/>
+      <c r="M8" s="130"/>
+      <c r="N8" s="130"/>
+      <c r="O8" s="130"/>
+      <c r="P8" s="130"/>
+      <c r="Q8" s="130"/>
+      <c r="R8" s="130"/>
+      <c r="S8" s="130"/>
+      <c r="T8" s="130"/>
+      <c r="U8" s="130"/>
+      <c r="V8" s="130"/>
+      <c r="W8" s="130"/>
+      <c r="X8" s="130"/>
+      <c r="Y8" s="130"/>
+      <c r="Z8" s="130"/>
+      <c r="AA8" s="130"/>
+      <c r="AB8" s="130"/>
+      <c r="AC8" s="130"/>
+      <c r="AD8" s="130"/>
+      <c r="AE8" s="130"/>
+      <c r="AF8" s="130"/>
+      <c r="AG8" s="131"/>
     </row>
     <row r="9" spans="1:33" ht="15.75" thickTop="1"/>
     <row r="10" spans="1:33" ht="15" customHeight="1">
@@ -2177,7 +2177,7 @@
       <c r="I10" s="119"/>
       <c r="J10" s="119"/>
       <c r="K10" s="120"/>
-      <c r="L10" s="121" t="s">
+      <c r="L10" s="118" t="s">
         <v>9</v>
       </c>
       <c r="M10" s="119"/>
@@ -2190,8 +2190,8 @@
       <c r="T10" s="119"/>
       <c r="U10" s="119"/>
       <c r="V10" s="120"/>
-      <c r="W10" s="121" t="s">
-        <v>59</v>
+      <c r="W10" s="118" t="s">
+        <v>58</v>
       </c>
       <c r="X10" s="119"/>
       <c r="Y10" s="119"/>
@@ -2216,7 +2216,7 @@
       <c r="I11" s="119"/>
       <c r="J11" s="119"/>
       <c r="K11" s="120"/>
-      <c r="L11" s="121"/>
+      <c r="L11" s="118"/>
       <c r="M11" s="119"/>
       <c r="N11" s="119"/>
       <c r="O11" s="119"/>
@@ -2227,7 +2227,7 @@
       <c r="T11" s="119"/>
       <c r="U11" s="119"/>
       <c r="V11" s="120"/>
-      <c r="W11" s="121"/>
+      <c r="W11" s="118"/>
       <c r="X11" s="119"/>
       <c r="Y11" s="119"/>
       <c r="Z11" s="119"/>
@@ -2240,45 +2240,45 @@
       <c r="AG11" s="120"/>
     </row>
     <row r="12" spans="1:33" ht="16.5" thickBot="1">
-      <c r="A12" s="116" t="s">
+      <c r="A12" s="114" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="117"/>
-      <c r="C12" s="117"/>
-      <c r="D12" s="117"/>
-      <c r="E12" s="117"/>
-      <c r="F12" s="117"/>
-      <c r="G12" s="117"/>
-      <c r="H12" s="117"/>
-      <c r="I12" s="117"/>
-      <c r="J12" s="117"/>
-      <c r="K12" s="118"/>
-      <c r="L12" s="117" t="s">
+      <c r="B12" s="112"/>
+      <c r="C12" s="112"/>
+      <c r="D12" s="112"/>
+      <c r="E12" s="112"/>
+      <c r="F12" s="112"/>
+      <c r="G12" s="112"/>
+      <c r="H12" s="112"/>
+      <c r="I12" s="112"/>
+      <c r="J12" s="112"/>
+      <c r="K12" s="113"/>
+      <c r="L12" s="112" t="s">
         <v>15</v>
       </c>
-      <c r="M12" s="117"/>
-      <c r="N12" s="117"/>
-      <c r="O12" s="117"/>
-      <c r="P12" s="117"/>
-      <c r="Q12" s="117"/>
-      <c r="R12" s="117"/>
-      <c r="S12" s="117"/>
-      <c r="T12" s="117"/>
-      <c r="U12" s="117"/>
-      <c r="V12" s="118"/>
-      <c r="W12" s="122" t="s">
+      <c r="M12" s="112"/>
+      <c r="N12" s="112"/>
+      <c r="O12" s="112"/>
+      <c r="P12" s="112"/>
+      <c r="Q12" s="112"/>
+      <c r="R12" s="112"/>
+      <c r="S12" s="112"/>
+      <c r="T12" s="112"/>
+      <c r="U12" s="112"/>
+      <c r="V12" s="113"/>
+      <c r="W12" s="111" t="s">
         <v>15</v>
       </c>
-      <c r="X12" s="117"/>
-      <c r="Y12" s="117"/>
-      <c r="Z12" s="117"/>
-      <c r="AA12" s="117"/>
-      <c r="AB12" s="117"/>
-      <c r="AC12" s="117"/>
-      <c r="AD12" s="117"/>
-      <c r="AE12" s="117"/>
-      <c r="AF12" s="117"/>
-      <c r="AG12" s="118"/>
+      <c r="X12" s="112"/>
+      <c r="Y12" s="112"/>
+      <c r="Z12" s="112"/>
+      <c r="AA12" s="112"/>
+      <c r="AB12" s="112"/>
+      <c r="AC12" s="112"/>
+      <c r="AD12" s="112"/>
+      <c r="AE12" s="112"/>
+      <c r="AF12" s="112"/>
+      <c r="AG12" s="113"/>
     </row>
     <row r="13" spans="1:33">
       <c r="A13" s="4"/>
@@ -2573,12 +2573,12 @@
       <c r="J17" s="4"/>
       <c r="K17" s="33"/>
       <c r="L17" s="4"/>
-      <c r="M17" s="123" t="s">
-        <v>77</v>
-      </c>
-      <c r="N17" s="123"/>
-      <c r="O17" s="123"/>
-      <c r="P17" s="123"/>
+      <c r="M17" s="121" t="s">
+        <v>76</v>
+      </c>
+      <c r="N17" s="121"/>
+      <c r="O17" s="121"/>
+      <c r="P17" s="121"/>
       <c r="Q17" s="8">
         <v>1</v>
       </c>
@@ -3073,12 +3073,12 @@
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
-      <c r="F23" s="106" t="s">
+      <c r="F23" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="G23" s="106"/>
-      <c r="H23" s="106"/>
-      <c r="I23" s="106"/>
+      <c r="G23" s="103"/>
+      <c r="H23" s="103"/>
+      <c r="I23" s="103"/>
       <c r="J23" s="4"/>
       <c r="K23" s="33"/>
       <c r="L23" s="4"/>
@@ -3086,12 +3086,12 @@
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
-      <c r="Q23" s="106" t="s">
+      <c r="Q23" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="R23" s="106"/>
-      <c r="S23" s="106"/>
-      <c r="T23" s="106"/>
+      <c r="R23" s="103"/>
+      <c r="S23" s="103"/>
+      <c r="T23" s="103"/>
       <c r="U23" s="4"/>
       <c r="V23" s="33"/>
       <c r="W23" s="4"/>
@@ -3099,12 +3099,12 @@
       <c r="Y23" s="4"/>
       <c r="Z23" s="4"/>
       <c r="AA23" s="4"/>
-      <c r="AB23" s="106" t="s">
+      <c r="AB23" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="AC23" s="106"/>
-      <c r="AD23" s="106"/>
-      <c r="AE23" s="106"/>
+      <c r="AC23" s="103"/>
+      <c r="AD23" s="103"/>
+      <c r="AE23" s="103"/>
       <c r="AF23" s="4"/>
       <c r="AG23" s="33"/>
     </row>
@@ -3144,45 +3144,45 @@
       <c r="AG24" s="33"/>
     </row>
     <row r="25" spans="1:33" ht="16.5" thickBot="1">
-      <c r="A25" s="116" t="s">
+      <c r="A25" s="114" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="117"/>
-      <c r="C25" s="117"/>
-      <c r="D25" s="117"/>
-      <c r="E25" s="117"/>
-      <c r="F25" s="117"/>
-      <c r="G25" s="117"/>
-      <c r="H25" s="117"/>
-      <c r="I25" s="117"/>
-      <c r="J25" s="117"/>
-      <c r="K25" s="118"/>
-      <c r="L25" s="122" t="s">
-        <v>57</v>
-      </c>
-      <c r="M25" s="117"/>
-      <c r="N25" s="117"/>
-      <c r="O25" s="117"/>
-      <c r="P25" s="117"/>
-      <c r="Q25" s="117"/>
-      <c r="R25" s="117"/>
-      <c r="S25" s="117"/>
-      <c r="T25" s="117"/>
-      <c r="U25" s="117"/>
-      <c r="V25" s="118"/>
-      <c r="W25" s="122" t="s">
+      <c r="B25" s="112"/>
+      <c r="C25" s="112"/>
+      <c r="D25" s="112"/>
+      <c r="E25" s="112"/>
+      <c r="F25" s="112"/>
+      <c r="G25" s="112"/>
+      <c r="H25" s="112"/>
+      <c r="I25" s="112"/>
+      <c r="J25" s="112"/>
+      <c r="K25" s="113"/>
+      <c r="L25" s="111" t="s">
+        <v>56</v>
+      </c>
+      <c r="M25" s="112"/>
+      <c r="N25" s="112"/>
+      <c r="O25" s="112"/>
+      <c r="P25" s="112"/>
+      <c r="Q25" s="112"/>
+      <c r="R25" s="112"/>
+      <c r="S25" s="112"/>
+      <c r="T25" s="112"/>
+      <c r="U25" s="112"/>
+      <c r="V25" s="113"/>
+      <c r="W25" s="111" t="s">
         <v>16</v>
       </c>
-      <c r="X25" s="117"/>
-      <c r="Y25" s="117"/>
-      <c r="Z25" s="117"/>
-      <c r="AA25" s="117"/>
-      <c r="AB25" s="117"/>
-      <c r="AC25" s="117"/>
-      <c r="AD25" s="117"/>
-      <c r="AE25" s="117"/>
-      <c r="AF25" s="117"/>
-      <c r="AG25" s="118"/>
+      <c r="X25" s="112"/>
+      <c r="Y25" s="112"/>
+      <c r="Z25" s="112"/>
+      <c r="AA25" s="112"/>
+      <c r="AB25" s="112"/>
+      <c r="AC25" s="112"/>
+      <c r="AD25" s="112"/>
+      <c r="AE25" s="112"/>
+      <c r="AF25" s="112"/>
+      <c r="AG25" s="113"/>
     </row>
     <row r="26" spans="1:33">
       <c r="A26" s="4"/>
@@ -3190,40 +3190,40 @@
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
-      <c r="F26" s="106" t="str">
+      <c r="F26" s="103" t="str">
         <f>F23</f>
         <v>world coordinates</v>
       </c>
-      <c r="G26" s="106"/>
-      <c r="H26" s="106"/>
-      <c r="I26" s="106"/>
+      <c r="G26" s="103"/>
+      <c r="H26" s="103"/>
+      <c r="I26" s="103"/>
       <c r="J26" s="4"/>
       <c r="K26" s="33"/>
-      <c r="L26" s="107" t="s">
-        <v>58</v>
-      </c>
-      <c r="M26" s="102"/>
-      <c r="N26" s="102"/>
-      <c r="O26" s="102"/>
-      <c r="P26" s="102"/>
-      <c r="Q26" s="102"/>
-      <c r="R26" s="102"/>
-      <c r="S26" s="102"/>
-      <c r="T26" s="102"/>
-      <c r="U26" s="102"/>
-      <c r="V26" s="108"/>
+      <c r="L26" s="104" t="s">
+        <v>57</v>
+      </c>
+      <c r="M26" s="105"/>
+      <c r="N26" s="105"/>
+      <c r="O26" s="105"/>
+      <c r="P26" s="105"/>
+      <c r="Q26" s="105"/>
+      <c r="R26" s="105"/>
+      <c r="S26" s="105"/>
+      <c r="T26" s="105"/>
+      <c r="U26" s="105"/>
+      <c r="V26" s="106"/>
       <c r="W26" s="4"/>
       <c r="X26" s="4"/>
       <c r="Y26" s="4"/>
       <c r="Z26" s="4"/>
       <c r="AA26" s="4"/>
-      <c r="AB26" s="106" t="str">
+      <c r="AB26" s="103" t="str">
         <f>AB23</f>
         <v>world coordinates</v>
       </c>
-      <c r="AC26" s="106"/>
-      <c r="AD26" s="106"/>
-      <c r="AE26" s="106"/>
+      <c r="AC26" s="103"/>
+      <c r="AD26" s="103"/>
+      <c r="AE26" s="103"/>
       <c r="AF26" s="4"/>
       <c r="AG26" s="33"/>
     </row>
@@ -3251,19 +3251,19 @@
       </c>
       <c r="J27" s="4"/>
       <c r="K27" s="33"/>
-      <c r="L27" s="107" t="s">
-        <v>70</v>
-      </c>
-      <c r="M27" s="102"/>
-      <c r="N27" s="102"/>
-      <c r="O27" s="102"/>
-      <c r="P27" s="102"/>
-      <c r="Q27" s="102"/>
-      <c r="R27" s="102"/>
-      <c r="S27" s="102"/>
-      <c r="T27" s="102"/>
-      <c r="U27" s="102"/>
-      <c r="V27" s="108"/>
+      <c r="L27" s="104" t="s">
+        <v>69</v>
+      </c>
+      <c r="M27" s="105"/>
+      <c r="N27" s="105"/>
+      <c r="O27" s="105"/>
+      <c r="P27" s="105"/>
+      <c r="Q27" s="105"/>
+      <c r="R27" s="105"/>
+      <c r="S27" s="105"/>
+      <c r="T27" s="105"/>
+      <c r="U27" s="105"/>
+      <c r="V27" s="106"/>
       <c r="W27" s="4"/>
       <c r="X27" s="4"/>
       <c r="Y27" s="4"/>
@@ -3312,18 +3312,18 @@
       </c>
       <c r="J28" s="4"/>
       <c r="K28" s="33"/>
-      <c r="L28" s="107" t="s">
-        <v>71</v>
-      </c>
-      <c r="M28" s="126"/>
-      <c r="N28" s="126"/>
-      <c r="O28" s="126"/>
-      <c r="P28" s="126"/>
-      <c r="Q28" s="126"/>
-      <c r="R28" s="126"/>
-      <c r="S28" s="126"/>
-      <c r="T28" s="126"/>
-      <c r="U28" s="126"/>
+      <c r="L28" s="104" t="s">
+        <v>70</v>
+      </c>
+      <c r="M28" s="117"/>
+      <c r="N28" s="117"/>
+      <c r="O28" s="117"/>
+      <c r="P28" s="117"/>
+      <c r="Q28" s="117"/>
+      <c r="R28" s="117"/>
+      <c r="S28" s="117"/>
+      <c r="T28" s="117"/>
+      <c r="U28" s="117"/>
       <c r="V28" s="33"/>
       <c r="W28" s="4"/>
       <c r="X28" s="2"/>
@@ -3373,19 +3373,19 @@
       </c>
       <c r="J29" s="4"/>
       <c r="K29" s="33"/>
-      <c r="L29" s="107" t="s">
-        <v>60</v>
-      </c>
-      <c r="M29" s="102"/>
-      <c r="N29" s="102"/>
-      <c r="O29" s="102"/>
-      <c r="P29" s="102"/>
-      <c r="Q29" s="102"/>
-      <c r="R29" s="102"/>
-      <c r="S29" s="102"/>
-      <c r="T29" s="102"/>
-      <c r="U29" s="102"/>
-      <c r="V29" s="108"/>
+      <c r="L29" s="104" t="s">
+        <v>59</v>
+      </c>
+      <c r="M29" s="105"/>
+      <c r="N29" s="105"/>
+      <c r="O29" s="105"/>
+      <c r="P29" s="105"/>
+      <c r="Q29" s="105"/>
+      <c r="R29" s="105"/>
+      <c r="S29" s="105"/>
+      <c r="T29" s="105"/>
+      <c r="U29" s="105"/>
+      <c r="V29" s="106"/>
       <c r="W29" s="4"/>
       <c r="X29" s="2"/>
       <c r="Y29" s="2"/>
@@ -3661,13 +3661,13 @@
       </c>
       <c r="J33" s="4"/>
       <c r="K33" s="33"/>
-      <c r="L33" s="124" t="s">
-        <v>54</v>
-      </c>
-      <c r="M33" s="125"/>
-      <c r="N33" s="125"/>
-      <c r="O33" s="125"/>
-      <c r="P33" s="125"/>
+      <c r="L33" s="115" t="s">
+        <v>53</v>
+      </c>
+      <c r="M33" s="116"/>
+      <c r="N33" s="116"/>
+      <c r="O33" s="116"/>
+      <c r="P33" s="116"/>
       <c r="Q33" s="21">
         <v>0</v>
       </c>
@@ -3989,12 +3989,12 @@
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
-      <c r="F37" s="106" t="s">
+      <c r="F37" s="103" t="s">
         <v>39</v>
       </c>
-      <c r="G37" s="106"/>
-      <c r="H37" s="106"/>
-      <c r="I37" s="106"/>
+      <c r="G37" s="103"/>
+      <c r="H37" s="103"/>
+      <c r="I37" s="103"/>
       <c r="J37" s="4"/>
       <c r="K37" s="33"/>
       <c r="L37" s="34"/>
@@ -4033,12 +4033,12 @@
       <c r="Y37" s="4"/>
       <c r="Z37" s="4"/>
       <c r="AA37" s="4"/>
-      <c r="AB37" s="106" t="s">
+      <c r="AB37" s="103" t="s">
         <v>39</v>
       </c>
-      <c r="AC37" s="106"/>
-      <c r="AD37" s="106"/>
-      <c r="AE37" s="106"/>
+      <c r="AC37" s="103"/>
+      <c r="AD37" s="103"/>
+      <c r="AE37" s="103"/>
       <c r="AF37" s="4"/>
       <c r="AG37" s="33"/>
     </row>
@@ -4059,12 +4059,12 @@
       <c r="N38" s="4"/>
       <c r="O38" s="4"/>
       <c r="P38" s="4"/>
-      <c r="Q38" s="106" t="s">
-        <v>55</v>
-      </c>
-      <c r="R38" s="106"/>
-      <c r="S38" s="106"/>
-      <c r="T38" s="106"/>
+      <c r="Q38" s="103" t="s">
+        <v>54</v>
+      </c>
+      <c r="R38" s="103"/>
+      <c r="S38" s="103"/>
+      <c r="T38" s="103"/>
       <c r="U38" s="4"/>
       <c r="V38" s="33"/>
       <c r="W38" s="4"/>
@@ -4080,19 +4080,19 @@
       <c r="AG38" s="33"/>
     </row>
     <row r="39" spans="1:33" ht="16.5" thickBot="1">
-      <c r="A39" s="116" t="s">
+      <c r="A39" s="114" t="s">
         <v>23</v>
       </c>
-      <c r="B39" s="117"/>
-      <c r="C39" s="117"/>
-      <c r="D39" s="117"/>
-      <c r="E39" s="117"/>
-      <c r="F39" s="117"/>
-      <c r="G39" s="117"/>
-      <c r="H39" s="117"/>
-      <c r="I39" s="117"/>
-      <c r="J39" s="117"/>
-      <c r="K39" s="118"/>
+      <c r="B39" s="112"/>
+      <c r="C39" s="112"/>
+      <c r="D39" s="112"/>
+      <c r="E39" s="112"/>
+      <c r="F39" s="112"/>
+      <c r="G39" s="112"/>
+      <c r="H39" s="112"/>
+      <c r="I39" s="112"/>
+      <c r="J39" s="112"/>
+      <c r="K39" s="113"/>
       <c r="L39" s="101"/>
       <c r="M39" s="4"/>
       <c r="N39" s="4"/>
@@ -4104,19 +4104,19 @@
       <c r="T39" s="4"/>
       <c r="U39" s="4"/>
       <c r="V39" s="33"/>
-      <c r="W39" s="122" t="s">
+      <c r="W39" s="111" t="s">
         <v>23</v>
       </c>
-      <c r="X39" s="117"/>
-      <c r="Y39" s="117"/>
-      <c r="Z39" s="117"/>
-      <c r="AA39" s="117"/>
-      <c r="AB39" s="117"/>
-      <c r="AC39" s="117"/>
-      <c r="AD39" s="117"/>
-      <c r="AE39" s="117"/>
-      <c r="AF39" s="117"/>
-      <c r="AG39" s="118"/>
+      <c r="X39" s="112"/>
+      <c r="Y39" s="112"/>
+      <c r="Z39" s="112"/>
+      <c r="AA39" s="112"/>
+      <c r="AB39" s="112"/>
+      <c r="AC39" s="112"/>
+      <c r="AD39" s="112"/>
+      <c r="AE39" s="112"/>
+      <c r="AF39" s="112"/>
+      <c r="AG39" s="113"/>
     </row>
     <row r="40" spans="1:33">
       <c r="A40" s="4"/>
@@ -4124,13 +4124,13 @@
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
-      <c r="F40" s="106" t="str">
+      <c r="F40" s="103" t="str">
         <f>F37</f>
         <v>eye coordinates</v>
       </c>
-      <c r="G40" s="106"/>
-      <c r="H40" s="106"/>
-      <c r="I40" s="106"/>
+      <c r="G40" s="103"/>
+      <c r="H40" s="103"/>
+      <c r="I40" s="103"/>
       <c r="J40" s="4"/>
       <c r="K40" s="33"/>
       <c r="L40" s="34"/>
@@ -4138,22 +4138,22 @@
       <c r="N40" s="4"/>
       <c r="O40" s="4"/>
       <c r="P40" s="4"/>
-      <c r="Q40" s="106" t="str">
+      <c r="Q40" s="103" t="str">
         <f>Q23</f>
         <v>world coordinates</v>
       </c>
-      <c r="R40" s="106"/>
-      <c r="S40" s="106"/>
-      <c r="T40" s="106"/>
+      <c r="R40" s="103"/>
+      <c r="S40" s="103"/>
+      <c r="T40" s="103"/>
       <c r="U40" s="4"/>
       <c r="V40" s="33"/>
-      <c r="AB40" s="106" t="str">
+      <c r="AB40" s="103" t="str">
         <f>AB23</f>
         <v>world coordinates</v>
       </c>
-      <c r="AC40" s="106"/>
-      <c r="AD40" s="106"/>
-      <c r="AE40" s="106"/>
+      <c r="AC40" s="103"/>
+      <c r="AD40" s="103"/>
+      <c r="AE40" s="103"/>
       <c r="AG40" s="33"/>
     </row>
     <row r="41" spans="1:33">
@@ -4517,7 +4517,7 @@
       <c r="J46" s="4"/>
       <c r="K46" s="33"/>
       <c r="L46" s="36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M46" s="13">
         <f>Q34</f>
@@ -4945,12 +4945,12 @@
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
-      <c r="F51" s="106" t="s">
+      <c r="F51" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="G51" s="106"/>
-      <c r="H51" s="106"/>
-      <c r="I51" s="106"/>
+      <c r="G51" s="103"/>
+      <c r="H51" s="103"/>
+      <c r="I51" s="103"/>
       <c r="J51" s="4"/>
       <c r="K51" s="33"/>
       <c r="L51" s="34"/>
@@ -4958,20 +4958,20 @@
       <c r="N51" s="4"/>
       <c r="O51" s="4"/>
       <c r="P51" s="4"/>
-      <c r="Q51" s="106" t="s">
+      <c r="Q51" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="R51" s="106"/>
-      <c r="S51" s="106"/>
-      <c r="T51" s="106"/>
+      <c r="R51" s="103"/>
+      <c r="S51" s="103"/>
+      <c r="T51" s="103"/>
       <c r="U51" s="4"/>
       <c r="V51" s="33"/>
-      <c r="AB51" s="106" t="s">
+      <c r="AB51" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="AC51" s="106"/>
-      <c r="AD51" s="106"/>
-      <c r="AE51" s="106"/>
+      <c r="AC51" s="103"/>
+      <c r="AD51" s="103"/>
+      <c r="AE51" s="103"/>
       <c r="AG51" s="33"/>
     </row>
     <row r="52" spans="1:33">
@@ -5000,51 +5000,51 @@
       <c r="AG52" s="33"/>
     </row>
     <row r="53" spans="1:33" ht="15.75">
-      <c r="A53" s="128" t="s">
+      <c r="A53" s="109" t="s">
         <v>34</v>
       </c>
-      <c r="B53" s="128"/>
-      <c r="C53" s="128"/>
-      <c r="D53" s="128"/>
-      <c r="E53" s="128"/>
-      <c r="F53" s="128"/>
-      <c r="G53" s="128"/>
-      <c r="H53" s="128"/>
-      <c r="I53" s="128"/>
-      <c r="J53" s="128"/>
-      <c r="K53" s="129"/>
-      <c r="L53" s="130" t="s">
+      <c r="B53" s="109"/>
+      <c r="C53" s="109"/>
+      <c r="D53" s="109"/>
+      <c r="E53" s="109"/>
+      <c r="F53" s="109"/>
+      <c r="G53" s="109"/>
+      <c r="H53" s="109"/>
+      <c r="I53" s="109"/>
+      <c r="J53" s="109"/>
+      <c r="K53" s="110"/>
+      <c r="L53" s="108" t="s">
         <v>34</v>
       </c>
-      <c r="M53" s="128"/>
-      <c r="N53" s="128"/>
-      <c r="O53" s="128"/>
-      <c r="P53" s="128"/>
-      <c r="Q53" s="128"/>
-      <c r="R53" s="128"/>
-      <c r="S53" s="128"/>
-      <c r="T53" s="128"/>
-      <c r="U53" s="128"/>
-      <c r="V53" s="129"/>
-      <c r="W53" s="130" t="s">
+      <c r="M53" s="109"/>
+      <c r="N53" s="109"/>
+      <c r="O53" s="109"/>
+      <c r="P53" s="109"/>
+      <c r="Q53" s="109"/>
+      <c r="R53" s="109"/>
+      <c r="S53" s="109"/>
+      <c r="T53" s="109"/>
+      <c r="U53" s="109"/>
+      <c r="V53" s="110"/>
+      <c r="W53" s="108" t="s">
         <v>34</v>
       </c>
-      <c r="X53" s="128"/>
-      <c r="Y53" s="128"/>
-      <c r="Z53" s="128"/>
-      <c r="AA53" s="128"/>
-      <c r="AB53" s="128"/>
-      <c r="AC53" s="128"/>
-      <c r="AD53" s="128"/>
-      <c r="AE53" s="128"/>
-      <c r="AF53" s="128"/>
-      <c r="AG53" s="129"/>
+      <c r="X53" s="109"/>
+      <c r="Y53" s="109"/>
+      <c r="Z53" s="109"/>
+      <c r="AA53" s="109"/>
+      <c r="AB53" s="109"/>
+      <c r="AC53" s="109"/>
+      <c r="AD53" s="109"/>
+      <c r="AE53" s="109"/>
+      <c r="AF53" s="109"/>
+      <c r="AG53" s="110"/>
     </row>
     <row r="54" spans="1:33">
-      <c r="A54" s="106"/>
-      <c r="B54" s="106"/>
-      <c r="C54" s="106"/>
-      <c r="D54" s="106"/>
+      <c r="A54" s="103"/>
+      <c r="B54" s="103"/>
+      <c r="C54" s="103"/>
+      <c r="D54" s="103"/>
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
       <c r="G54" s="4"/>
@@ -5052,10 +5052,10 @@
       <c r="I54" s="4"/>
       <c r="J54" s="4"/>
       <c r="K54" s="33"/>
-      <c r="L54" s="127"/>
-      <c r="M54" s="106"/>
-      <c r="N54" s="106"/>
-      <c r="O54" s="106"/>
+      <c r="L54" s="102"/>
+      <c r="M54" s="103"/>
+      <c r="N54" s="103"/>
+      <c r="O54" s="103"/>
       <c r="P54" s="4"/>
       <c r="Q54" s="4"/>
       <c r="R54" s="4"/>
@@ -5063,10 +5063,10 @@
       <c r="T54" s="4"/>
       <c r="U54" s="4"/>
       <c r="V54" s="33"/>
-      <c r="W54" s="127"/>
-      <c r="X54" s="106"/>
-      <c r="Y54" s="106"/>
-      <c r="Z54" s="106"/>
+      <c r="W54" s="102"/>
+      <c r="X54" s="103"/>
+      <c r="Y54" s="103"/>
+      <c r="Z54" s="103"/>
       <c r="AA54" s="4"/>
       <c r="AB54" s="4"/>
       <c r="AC54" s="4"/>
@@ -5401,50 +5401,50 @@
       <c r="AG59" s="33"/>
     </row>
     <row r="60" spans="1:33">
-      <c r="A60" s="106" t="s">
+      <c r="A60" s="103" t="s">
         <v>41</v>
       </c>
-      <c r="B60" s="106"/>
-      <c r="C60" s="106"/>
-      <c r="D60" s="106"/>
-      <c r="E60" s="102" t="s">
-        <v>76</v>
-      </c>
-      <c r="F60" s="102"/>
-      <c r="G60" s="102"/>
-      <c r="H60" s="102"/>
-      <c r="I60" s="102"/>
-      <c r="J60" s="102"/>
+      <c r="B60" s="103"/>
+      <c r="C60" s="103"/>
+      <c r="D60" s="103"/>
+      <c r="E60" s="105" t="s">
+        <v>75</v>
+      </c>
+      <c r="F60" s="105"/>
+      <c r="G60" s="105"/>
+      <c r="H60" s="105"/>
+      <c r="I60" s="105"/>
+      <c r="J60" s="105"/>
       <c r="K60" s="33"/>
-      <c r="L60" s="127" t="s">
+      <c r="L60" s="102" t="s">
         <v>41</v>
       </c>
-      <c r="M60" s="106"/>
-      <c r="N60" s="106"/>
-      <c r="O60" s="106"/>
-      <c r="P60" s="102" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q60" s="102"/>
-      <c r="R60" s="102"/>
-      <c r="S60" s="102"/>
-      <c r="T60" s="102"/>
-      <c r="U60" s="102"/>
+      <c r="M60" s="103"/>
+      <c r="N60" s="103"/>
+      <c r="O60" s="103"/>
+      <c r="P60" s="105" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q60" s="105"/>
+      <c r="R60" s="105"/>
+      <c r="S60" s="105"/>
+      <c r="T60" s="105"/>
+      <c r="U60" s="105"/>
       <c r="V60" s="33"/>
-      <c r="W60" s="127" t="s">
+      <c r="W60" s="102" t="s">
         <v>41</v>
       </c>
-      <c r="X60" s="106"/>
-      <c r="Y60" s="106"/>
-      <c r="Z60" s="106"/>
-      <c r="AA60" s="102" t="s">
-        <v>76</v>
-      </c>
-      <c r="AB60" s="102"/>
-      <c r="AC60" s="102"/>
-      <c r="AD60" s="102"/>
-      <c r="AE60" s="102"/>
-      <c r="AF60" s="102"/>
+      <c r="X60" s="103"/>
+      <c r="Y60" s="103"/>
+      <c r="Z60" s="103"/>
+      <c r="AA60" s="105" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB60" s="105"/>
+      <c r="AC60" s="105"/>
+      <c r="AD60" s="105"/>
+      <c r="AE60" s="105"/>
+      <c r="AF60" s="105"/>
       <c r="AG60" s="33"/>
     </row>
     <row r="61" spans="1:33">
@@ -5514,54 +5514,54 @@
       <c r="AG62" s="33"/>
     </row>
     <row r="63" spans="1:33" ht="16.5" thickBot="1">
-      <c r="A63" s="116" t="s">
+      <c r="A63" s="114" t="s">
         <v>47</v>
       </c>
-      <c r="B63" s="117"/>
-      <c r="C63" s="117"/>
-      <c r="D63" s="117"/>
-      <c r="E63" s="117"/>
-      <c r="F63" s="117"/>
-      <c r="G63" s="117"/>
-      <c r="H63" s="117"/>
-      <c r="I63" s="117"/>
-      <c r="J63" s="117"/>
-      <c r="K63" s="118"/>
-      <c r="L63" s="122" t="s">
+      <c r="B63" s="112"/>
+      <c r="C63" s="112"/>
+      <c r="D63" s="112"/>
+      <c r="E63" s="112"/>
+      <c r="F63" s="112"/>
+      <c r="G63" s="112"/>
+      <c r="H63" s="112"/>
+      <c r="I63" s="112"/>
+      <c r="J63" s="112"/>
+      <c r="K63" s="113"/>
+      <c r="L63" s="111" t="s">
         <v>47</v>
       </c>
-      <c r="M63" s="117"/>
-      <c r="N63" s="117"/>
-      <c r="O63" s="117"/>
-      <c r="P63" s="117"/>
-      <c r="Q63" s="117"/>
-      <c r="R63" s="117"/>
-      <c r="S63" s="117"/>
-      <c r="T63" s="117"/>
-      <c r="U63" s="117"/>
-      <c r="V63" s="118"/>
-      <c r="W63" s="122" t="s">
+      <c r="M63" s="112"/>
+      <c r="N63" s="112"/>
+      <c r="O63" s="112"/>
+      <c r="P63" s="112"/>
+      <c r="Q63" s="112"/>
+      <c r="R63" s="112"/>
+      <c r="S63" s="112"/>
+      <c r="T63" s="112"/>
+      <c r="U63" s="112"/>
+      <c r="V63" s="113"/>
+      <c r="W63" s="111" t="s">
         <v>47</v>
       </c>
-      <c r="X63" s="117"/>
-      <c r="Y63" s="117"/>
-      <c r="Z63" s="117"/>
-      <c r="AA63" s="117"/>
-      <c r="AB63" s="117"/>
-      <c r="AC63" s="117"/>
-      <c r="AD63" s="117"/>
-      <c r="AE63" s="117"/>
-      <c r="AF63" s="117"/>
-      <c r="AG63" s="118"/>
+      <c r="X63" s="112"/>
+      <c r="Y63" s="112"/>
+      <c r="Z63" s="112"/>
+      <c r="AA63" s="112"/>
+      <c r="AB63" s="112"/>
+      <c r="AC63" s="112"/>
+      <c r="AD63" s="112"/>
+      <c r="AE63" s="112"/>
+      <c r="AF63" s="112"/>
+      <c r="AG63" s="113"/>
     </row>
     <row r="64" spans="1:33">
-      <c r="A64" s="106" t="str">
+      <c r="A64" s="103" t="str">
         <f>A60</f>
         <v>normalized device coordinates</v>
       </c>
-      <c r="B64" s="106"/>
-      <c r="C64" s="106"/>
-      <c r="D64" s="106"/>
+      <c r="B64" s="103"/>
+      <c r="C64" s="103"/>
+      <c r="D64" s="103"/>
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
       <c r="G64" s="4"/>
@@ -5569,13 +5569,13 @@
       <c r="I64" s="4"/>
       <c r="J64" s="4"/>
       <c r="K64" s="33"/>
-      <c r="L64" s="127" t="str">
+      <c r="L64" s="102" t="str">
         <f>L60</f>
         <v>normalized device coordinates</v>
       </c>
-      <c r="M64" s="106"/>
-      <c r="N64" s="106"/>
-      <c r="O64" s="106"/>
+      <c r="M64" s="103"/>
+      <c r="N64" s="103"/>
+      <c r="O64" s="103"/>
       <c r="P64" s="4"/>
       <c r="Q64" s="4"/>
       <c r="R64" s="4"/>
@@ -5583,13 +5583,13 @@
       <c r="T64" s="4"/>
       <c r="U64" s="4"/>
       <c r="V64" s="33"/>
-      <c r="W64" s="127" t="str">
+      <c r="W64" s="102" t="str">
         <f>W60</f>
         <v>normalized device coordinates</v>
       </c>
-      <c r="X64" s="106"/>
-      <c r="Y64" s="106"/>
-      <c r="Z64" s="106"/>
+      <c r="X64" s="103"/>
+      <c r="Y64" s="103"/>
+      <c r="Z64" s="103"/>
       <c r="AA64" s="4"/>
       <c r="AB64" s="4"/>
       <c r="AC64" s="4"/>
@@ -5607,15 +5607,15 @@
         <v>2</v>
       </c>
       <c r="D65" s="97" t="s">
-        <v>78</v>
-      </c>
-      <c r="E65" s="103" t="s">
-        <v>67</v>
-      </c>
-      <c r="F65" s="103"/>
-      <c r="G65" s="103"/>
+        <v>77</v>
+      </c>
+      <c r="E65" s="123" t="s">
+        <v>66</v>
+      </c>
+      <c r="F65" s="123"/>
+      <c r="G65" s="123"/>
       <c r="H65" s="67" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I65" s="66">
         <v>-1</v>
@@ -5630,15 +5630,15 @@
         <v>2</v>
       </c>
       <c r="O65" s="97" t="s">
-        <v>78</v>
-      </c>
-      <c r="P65" s="103" t="s">
+        <v>77</v>
+      </c>
+      <c r="P65" s="123" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q65" s="123"/>
+      <c r="R65" s="123"/>
+      <c r="S65" s="67" t="s">
         <v>68</v>
-      </c>
-      <c r="Q65" s="103"/>
-      <c r="R65" s="103"/>
-      <c r="S65" s="67" t="s">
-        <v>69</v>
       </c>
       <c r="T65" s="66">
         <v>1</v>
@@ -5653,15 +5653,15 @@
         <v>2</v>
       </c>
       <c r="Z65" s="97" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA65" s="103" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB65" s="103"/>
-      <c r="AC65" s="103"/>
+        <v>77</v>
+      </c>
+      <c r="AA65" s="123" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB65" s="123"/>
+      <c r="AC65" s="123"/>
       <c r="AD65" s="67" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AE65" s="68">
         <v>-1</v>
@@ -5978,50 +5978,50 @@
       <c r="AG69" s="33"/>
     </row>
     <row r="70" spans="1:33">
-      <c r="A70" s="106" t="s">
+      <c r="A70" s="103" t="s">
         <v>48</v>
       </c>
-      <c r="B70" s="106"/>
-      <c r="C70" s="106"/>
-      <c r="D70" s="106"/>
-      <c r="E70" s="102" t="s">
-        <v>79</v>
-      </c>
-      <c r="F70" s="102"/>
-      <c r="G70" s="102"/>
-      <c r="H70" s="102"/>
-      <c r="I70" s="102"/>
-      <c r="J70" s="102"/>
+      <c r="B70" s="103"/>
+      <c r="C70" s="103"/>
+      <c r="D70" s="103"/>
+      <c r="E70" s="105" t="s">
+        <v>78</v>
+      </c>
+      <c r="F70" s="105"/>
+      <c r="G70" s="105"/>
+      <c r="H70" s="105"/>
+      <c r="I70" s="105"/>
+      <c r="J70" s="105"/>
       <c r="K70" s="33"/>
-      <c r="L70" s="127" t="s">
+      <c r="L70" s="102" t="s">
         <v>48</v>
       </c>
-      <c r="M70" s="106"/>
-      <c r="N70" s="106"/>
-      <c r="O70" s="106"/>
-      <c r="P70" s="102" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q70" s="102"/>
-      <c r="R70" s="102"/>
-      <c r="S70" s="102"/>
-      <c r="T70" s="102"/>
-      <c r="U70" s="102"/>
+      <c r="M70" s="103"/>
+      <c r="N70" s="103"/>
+      <c r="O70" s="103"/>
+      <c r="P70" s="105" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q70" s="105"/>
+      <c r="R70" s="105"/>
+      <c r="S70" s="105"/>
+      <c r="T70" s="105"/>
+      <c r="U70" s="105"/>
       <c r="V70" s="33"/>
-      <c r="W70" s="127" t="s">
+      <c r="W70" s="102" t="s">
         <v>48</v>
       </c>
-      <c r="X70" s="106"/>
-      <c r="Y70" s="106"/>
-      <c r="Z70" s="106"/>
-      <c r="AA70" s="102" t="s">
-        <v>79</v>
-      </c>
-      <c r="AB70" s="102"/>
-      <c r="AC70" s="102"/>
-      <c r="AD70" s="102"/>
-      <c r="AE70" s="102"/>
-      <c r="AF70" s="102"/>
+      <c r="X70" s="103"/>
+      <c r="Y70" s="103"/>
+      <c r="Z70" s="103"/>
+      <c r="AA70" s="105" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB70" s="105"/>
+      <c r="AC70" s="105"/>
+      <c r="AD70" s="105"/>
+      <c r="AE70" s="105"/>
+      <c r="AF70" s="105"/>
       <c r="AG70" s="33"/>
     </row>
     <row r="71" spans="1:33">
@@ -6946,6 +6946,63 @@
     </row>
   </sheetData>
   <mergeCells count="73">
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="E70:J70"/>
+    <mergeCell ref="P70:U70"/>
+    <mergeCell ref="AA70:AF70"/>
+    <mergeCell ref="E60:J60"/>
+    <mergeCell ref="P60:U60"/>
+    <mergeCell ref="AA60:AF60"/>
+    <mergeCell ref="AA65:AC65"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="L26:V26"/>
+    <mergeCell ref="L27:V27"/>
+    <mergeCell ref="Q38:T38"/>
+    <mergeCell ref="Q40:T40"/>
+    <mergeCell ref="Q51:T51"/>
+    <mergeCell ref="G1:T1"/>
+    <mergeCell ref="E65:G65"/>
+    <mergeCell ref="P65:R65"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="A8:AG8"/>
+    <mergeCell ref="A64:D64"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="F51:I51"/>
+    <mergeCell ref="A60:D60"/>
+    <mergeCell ref="A39:K39"/>
+    <mergeCell ref="A10:K11"/>
+    <mergeCell ref="A12:K12"/>
+    <mergeCell ref="A25:K25"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="L10:V11"/>
+    <mergeCell ref="W10:AG11"/>
+    <mergeCell ref="L12:V12"/>
+    <mergeCell ref="Q23:T23"/>
+    <mergeCell ref="L25:V25"/>
+    <mergeCell ref="M17:P17"/>
+    <mergeCell ref="L33:P33"/>
+    <mergeCell ref="L28:U28"/>
+    <mergeCell ref="W12:AG12"/>
+    <mergeCell ref="AB23:AE23"/>
+    <mergeCell ref="W25:AG25"/>
+    <mergeCell ref="L64:O64"/>
+    <mergeCell ref="L70:O70"/>
+    <mergeCell ref="L54:O54"/>
+    <mergeCell ref="A53:K53"/>
+    <mergeCell ref="A63:K63"/>
+    <mergeCell ref="L53:V53"/>
+    <mergeCell ref="A70:D70"/>
+    <mergeCell ref="A54:D54"/>
     <mergeCell ref="W70:Z70"/>
     <mergeCell ref="L29:V29"/>
     <mergeCell ref="S2:T2"/>
@@ -6962,63 +7019,6 @@
     <mergeCell ref="W39:AG39"/>
     <mergeCell ref="L60:O60"/>
     <mergeCell ref="L63:V63"/>
-    <mergeCell ref="L64:O64"/>
-    <mergeCell ref="L70:O70"/>
-    <mergeCell ref="L54:O54"/>
-    <mergeCell ref="A53:K53"/>
-    <mergeCell ref="A63:K63"/>
-    <mergeCell ref="L53:V53"/>
-    <mergeCell ref="A70:D70"/>
-    <mergeCell ref="A54:D54"/>
-    <mergeCell ref="L33:P33"/>
-    <mergeCell ref="L28:U28"/>
-    <mergeCell ref="W12:AG12"/>
-    <mergeCell ref="AB23:AE23"/>
-    <mergeCell ref="W25:AG25"/>
-    <mergeCell ref="L10:V11"/>
-    <mergeCell ref="W10:AG11"/>
-    <mergeCell ref="L12:V12"/>
-    <mergeCell ref="Q23:T23"/>
-    <mergeCell ref="L25:V25"/>
-    <mergeCell ref="M17:P17"/>
-    <mergeCell ref="A39:K39"/>
-    <mergeCell ref="A10:K11"/>
-    <mergeCell ref="A12:K12"/>
-    <mergeCell ref="A25:K25"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="G1:T1"/>
-    <mergeCell ref="E65:G65"/>
-    <mergeCell ref="P65:R65"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="A8:AG8"/>
-    <mergeCell ref="A64:D64"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="F51:I51"/>
-    <mergeCell ref="A60:D60"/>
-    <mergeCell ref="W2:X2"/>
-    <mergeCell ref="E70:J70"/>
-    <mergeCell ref="P70:U70"/>
-    <mergeCell ref="AA70:AF70"/>
-    <mergeCell ref="E60:J60"/>
-    <mergeCell ref="P60:U60"/>
-    <mergeCell ref="AA60:AF60"/>
-    <mergeCell ref="AA65:AC65"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="L26:V26"/>
-    <mergeCell ref="L27:V27"/>
-    <mergeCell ref="Q38:T38"/>
-    <mergeCell ref="Q40:T40"/>
-    <mergeCell ref="Q51:T51"/>
   </mergeCells>
   <conditionalFormatting sqref="E66:E69 P66:P69 AA66:AA69">
     <cfRule type="containsText" dxfId="7" priority="10" operator="containsText" text="FAIL">

</xml_diff>